<commit_message>
add calculated weighted scenario to output
</commit_message>
<xml_diff>
--- a/data/SCENARIOS.xlsx
+++ b/data/SCENARIOS.xlsx
@@ -8,16 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\geyerbisschoff\PythonProjects\Z-model\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3EE41FC-87A3-4C24-A276-AF69E8392871}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3ED0FF7-98D4-4453-BC17-150A03736767}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-40212" yWindow="-6528" windowWidth="40320" windowHeight="17496" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-40212" yWindow="-6528" windowWidth="40320" windowHeight="17496" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DATA" sheetId="4" r:id="rId1"/>
-    <sheet name="CONSTANTS" sheetId="2" state="hidden" r:id="rId2"/>
+    <sheet name="SCENARIO_WEIGHTS" sheetId="5" r:id="rId2"/>
+    <sheet name="CONSTANTS" sheetId="2" state="hidden" r:id="rId3"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId3"/>
+    <externalReference r:id="rId4"/>
   </externalReferences>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">DATA!$A$1:$E$580</definedName>
@@ -25,7 +26,7 @@
     <definedName name="_QUATER">CONSTANTS!$B$2:$B$5</definedName>
     <definedName name="Date_Reporting">[1]Inputs!$D$2</definedName>
   </definedNames>
-  <calcPr calcId="191029" calcOnSave="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -44,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="604" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="609" uniqueCount="29">
   <si>
     <t>SCENARIO</t>
   </si>
@@ -129,12 +130,15 @@
   <si>
     <t>INDEX</t>
   </si>
+  <si>
+    <t>WEIGHT</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -165,6 +169,13 @@
     </font>
     <font>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -231,11 +242,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -252,10 +264,14 @@
     <xf numFmtId="14" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -5067,8 +5083,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G580"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19967,6 +19983,58 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C987694D-C94C-4105-A6ED-DDE0EF8B3EDF}">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.5703125" customWidth="1"/>
+    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" s="6">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" s="6">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" s="6">
+        <v>0.3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B13"/>
   <sheetViews>

</xml_diff>